<commit_message>
Chnages on 22-March-24 added the data in tis commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestExcel.xlsx
+++ b/src/test/resources/TestExcel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Testcases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
   <si>
     <t>LoginTest</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Automation4</t>
+  </si>
+  <si>
+    <t>RegisterationTest</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -523,7 +528,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -554,7 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>

</xml_diff>